<commit_message>
(#222)  Correct expected counts.
</commit_message>
<xml_diff>
--- a/test-data/pdq-citations-data.xlsx
+++ b/test-data/pdq-citations-data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C525DA75-1A20-4E3B-A528-44A126480CA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1FEAD6-AF69-3542-8270-12075A075025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="4140" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_pdq_citations" sheetId="1" r:id="rId1"/>
@@ -570,16 +570,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="88.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="88.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -597,7 +597,7 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -611,10 +611,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -631,7 +631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -648,7 +648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -665,7 +665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>55</v>
       </c>
@@ -696,13 +696,13 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="88.85546875" customWidth="1"/>
+    <col min="1" max="1" width="88.83203125" customWidth="1"/>
     <col min="2" max="2" width="138" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -713,7 +713,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -724,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>51</v>
       </c>
@@ -768,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>51</v>
       </c>
@@ -779,7 +779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>52</v>
       </c>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>52</v>
       </c>
@@ -801,7 +801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>52</v>
       </c>
@@ -812,7 +812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>55</v>
       </c>
@@ -824,7 +824,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>55</v>
       </c>
@@ -835,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>55</v>
       </c>
@@ -871,18 +871,19 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.28515625" customWidth="1"/>
+    <col min="1" max="1" width="71.33203125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -902,7 +903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -916,13 +917,13 @@
         <v>7</v>
       </c>
       <c r="E2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -942,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>51</v>
       </c>
@@ -962,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>52</v>
       </c>
@@ -982,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>55</v>
       </c>
@@ -1016,14 +1017,14 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.140625" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="1" max="1" width="70.1640625" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1034,7 +1035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1056,7 +1057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1078,7 +1079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1100,7 +1101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1111,7 +1112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1122,7 +1123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -1166,7 +1167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -1177,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>35</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
@@ -1221,7 +1222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>41</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>43</v>
       </c>
@@ -1243,7 +1244,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>44</v>
       </c>
@@ -1254,7 +1255,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>45</v>
       </c>
@@ -1265,7 +1266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>47</v>
       </c>
@@ -1276,7 +1277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>48</v>
       </c>

</xml_diff>